<commit_message>
Improved Exception Habdling , and Transaction item OutPut
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -689,8 +689,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1775,8 +1775,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1826,7 +1826,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>
@@ -1837,7 +1837,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Config and SQL updated
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -254,9 +254,6 @@
     <t>Dsn=voltas</t>
   </si>
   <si>
-    <t>&lt;Mid,&gt;Mid, MNPR  -- -   290,300,250</t>
-  </si>
-  <si>
     <t>https://vcare.voltasworld.com/siebel/app/htim/enu?SWECmd=GotoView&amp;SWEView=CUT+Home+Page+View+(CME)&amp;SWERF=1&amp;SWEHo=vcare.voltasworld.com&amp;SWEBU=1&amp;SWEApplet0=Salutation+Applet+(WCC+Home)&amp;SWERowId0=VRId-0</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>VoltasNonStandardExpenseAutomationRE</t>
+  </si>
+  <si>
+    <t>&lt;Mid-MJPR   ,    &gt;Mid-MPPR    ,     &lt;Mid-MNPR    ,     &gt;Mid-MNPR  ---   290,300,250,290</t>
   </si>
 </sst>
 </file>
@@ -317,10 +317,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF464E55"/>
-      <name val="Segoe UI"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -362,7 +363,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -372,6 +372,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,7 +764,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
@@ -1849,7 +1850,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1971,7 +1972,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1982,10 +1983,10 @@
       <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C23" s="12"/>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
@@ -1994,10 +1995,10 @@
       <c r="B24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C25" s="12"/>
+      <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
@@ -2006,10 +2007,10 @@
       <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="12"/>
+      <c r="C26" s="11"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C27" s="12"/>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="2" t="s">
@@ -2018,7 +2019,7 @@
       <c r="B28" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="12"/>
+      <c r="C28" s="11"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
@@ -2028,15 +2029,15 @@
       <c r="B30" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C31" s="12"/>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C32" s="12"/>
+      <c r="C32" s="11"/>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
@@ -2045,7 +2046,7 @@
       <c r="B33" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="12"/>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
@@ -2055,12 +2056,12 @@
       <c r="B35" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C36" s="12"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -2069,7 +2070,7 @@
       <c r="B37" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="12"/>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2080,13 +2081,13 @@
       <c r="B40" s="6">
         <v>20</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="B41" s="6"/>
-      <c r="C41" s="12"/>
+      <c r="C41" s="11"/>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="2" t="s">
@@ -2095,11 +2096,11 @@
       <c r="B42" s="6">
         <v>40</v>
       </c>
-      <c r="C42" s="12"/>
+      <c r="C42" s="11"/>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="B43" s="6"/>
-      <c r="C43" s="12"/>
+      <c r="C43" s="11"/>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" s="2" t="s">
@@ -2108,15 +2109,15 @@
       <c r="B44" s="6">
         <v>75</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="11"/>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" t="s">
         <v>79</v>
-      </c>
-      <c r="B46" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3079,8 +3080,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3088,7 +3089,8 @@
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="4" max="4" width="95" customWidth="1"/>
+    <col min="5" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3137,8 +3139,8 @@
       <c r="C2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>76</v>
+      <c r="D2" s="10" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3158,7 +3160,7 @@
         <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3177,7 +3179,7 @@
       <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="13" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dealer Explanation and Expense amount Updated
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>&lt;Mid-MJPR   ,    &gt;Mid-MPPR    ,     &lt;Mid-MNPR    ,     &gt;Mid-MNPR  ---   290,300,250,290</t>
+  </si>
+  <si>
+    <t>MinDistanceMJPRGMinus</t>
   </si>
 </sst>
 </file>
@@ -366,13 +369,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1776,8 +1779,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1972,7 +1975,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1983,10 +1986,10 @@
       <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C23" s="11"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
@@ -1995,10 +1998,10 @@
       <c r="B24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C25" s="11"/>
+      <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
@@ -2007,10 +2010,10 @@
       <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C27" s="11"/>
+      <c r="C27" s="12"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="2" t="s">
@@ -2019,7 +2022,7 @@
       <c r="B28" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
@@ -2029,15 +2032,15 @@
       <c r="B30" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C31" s="11"/>
+      <c r="C31" s="12"/>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C32" s="11"/>
+      <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
@@ -2046,7 +2049,7 @@
       <c r="B33" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
@@ -2056,12 +2059,12 @@
       <c r="B35" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C36" s="11"/>
+      <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -2070,7 +2073,7 @@
       <c r="B37" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="11"/>
+      <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2081,13 +2084,13 @@
       <c r="B40" s="6">
         <v>20</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="B41" s="6"/>
-      <c r="C41" s="11"/>
+      <c r="C41" s="12"/>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="2" t="s">
@@ -2096,11 +2099,11 @@
       <c r="B42" s="6">
         <v>40</v>
       </c>
-      <c r="C42" s="11"/>
+      <c r="C42" s="12"/>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="B43" s="6"/>
-      <c r="C43" s="11"/>
+      <c r="C43" s="12"/>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" s="2" t="s">
@@ -2109,7 +2112,7 @@
       <c r="B44" s="6">
         <v>75</v>
       </c>
-      <c r="C44" s="11"/>
+      <c r="C44" s="12"/>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
@@ -2121,7 +2124,14 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A48" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48">
+        <v>40</v>
+      </c>
+    </row>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -3080,8 +3090,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3179,7 +3189,7 @@
       <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Expense Amount Logic Changed, and Dealer Remarks changed for Business Rule Exception Expense Order ID's
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="1"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -152,9 +152,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>majorgas</t>
-  </si>
-  <si>
     <t>Shared/Non_stand</t>
   </si>
   <si>
@@ -248,9 +245,6 @@
     <t>{"DB","MJGAS"} DB for DB Rates , MJGAS for Major gas Rates</t>
   </si>
   <si>
-    <t>CustAmount</t>
-  </si>
-  <si>
     <t>Dsn=voltas</t>
   </si>
   <si>
@@ -269,17 +263,41 @@
     <t>VoltasNonStandardExpenseAutomationRE</t>
   </si>
   <si>
-    <t>&lt;Mid-MJPR   ,    &gt;Mid-MPPR    ,     &lt;Mid-MNPR    ,     &gt;Mid-MNPR  ---   290,300,250,290</t>
-  </si>
-  <si>
     <t>MinDistanceMJPRGMinus</t>
+  </si>
+  <si>
+    <t>MinDistanceMNPRMinus</t>
+  </si>
+  <si>
+    <t>SrNotFoundStypeErr</t>
+  </si>
+  <si>
+    <t>Delete this Exps - Uipath Error</t>
+  </si>
+  <si>
+    <t>AmountMJPRWGC</t>
+  </si>
+  <si>
+    <t>&lt;Min , &gt;Min &lt; mid , &gt;Mid &lt; max , &gt;Max   =  250,250,290,350</t>
+  </si>
+  <si>
+    <t>AmountMJPR</t>
+  </si>
+  <si>
+    <t>&lt;Min , &gt;Min &lt; mid , &gt;Mid &lt; max , &gt;Max   =  150,150,250,350</t>
+  </si>
+  <si>
+    <t>AmountMNPR</t>
+  </si>
+  <si>
+    <t>&lt;Min , &gt;Min &lt; mid , &gt;Mid &lt; max , &gt;Max   =  150,150,250,290</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -326,6 +344,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF464E55"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -347,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -366,15 +390,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,8 +718,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -744,7 +769,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -755,7 +780,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -767,7 +792,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
@@ -1779,8 +1804,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1853,7 +1878,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1965,189 +1990,203 @@
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="6">
         <v>50</v>
       </c>
       <c r="C20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="C21" s="11" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C21" s="12" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C23" s="12"/>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="12"/>
+        <v>48</v>
+      </c>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C25" s="12"/>
+      <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="12"/>
+        <v>49</v>
+      </c>
+      <c r="C26" s="11"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C27" s="12"/>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
         <v>54</v>
       </c>
-      <c r="B28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="12"/>
+      <c r="C28" s="11"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C31" s="12"/>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C32" s="12"/>
+      <c r="C32" s="11"/>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" t="s">
         <v>64</v>
       </c>
-      <c r="B35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>63</v>
+      <c r="C35" s="12" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C36" s="12"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40" s="6">
-        <v>20</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>70</v>
+        <v>25</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="B41" s="6"/>
-      <c r="C41" s="12"/>
+      <c r="C41" s="11"/>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" s="6">
-        <v>40</v>
-      </c>
-      <c r="C42" s="12"/>
+        <v>50</v>
+      </c>
+      <c r="C42" s="11"/>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="B43" s="6"/>
-      <c r="C43" s="12"/>
+      <c r="C43" s="11"/>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B44" s="6">
         <v>75</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="11"/>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B48">
         <v>40</v>
       </c>
     </row>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="49" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="50" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="52" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="56" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="57" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="58" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="59" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="60" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -3088,10 +3127,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3141,36 +3180,36 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>76</v>
+        <v>42</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3181,16 +3220,16 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>46</v>
+        <v>70</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>75</v>
+        <v>42</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -3200,28 +3239,49 @@
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>72</v>
+      <c r="A8" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>42</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4211,8 +4271,6 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
-    <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new chanages regarding srinivasa ele
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>&lt;Min , &gt;Min &lt; mid , &gt;Mid &lt; max , &gt;Max   =  150,150,250,290</t>
+  </si>
+  <si>
+    <t>DescriptionPolicy</t>
+  </si>
+  <si>
+    <t>Dealer Remarks</t>
   </si>
 </sst>
 </file>
@@ -391,15 +397,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,7 +724,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1804,8 +1810,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2000,7 +2006,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="13" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2011,10 +2017,10 @@
       <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="13"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C23" s="11"/>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
@@ -2023,10 +2029,10 @@
       <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="13"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C25" s="11"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
@@ -2035,10 +2041,10 @@
       <c r="B26" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C27" s="11"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="2" t="s">
@@ -2047,7 +2053,7 @@
       <c r="B28" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
@@ -2057,15 +2063,15 @@
       <c r="B30" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C31" s="11"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C32" s="11"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
@@ -2074,7 +2080,7 @@
       <c r="B33" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
@@ -2084,12 +2090,12 @@
       <c r="B35" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C36" s="11"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" s="2" t="s">
@@ -2098,7 +2104,7 @@
       <c r="B37" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="11"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2109,35 +2115,35 @@
       <c r="B40" s="6">
         <v>25</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="14" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="B41" s="6"/>
-      <c r="C41" s="11"/>
+      <c r="C41" s="13"/>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B42" s="6">
-        <v>50</v>
-      </c>
-      <c r="C42" s="11"/>
+        <v>49</v>
+      </c>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="B43" s="6"/>
-      <c r="C43" s="11"/>
+      <c r="C43" s="13"/>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B44" s="6">
-        <v>75</v>
-      </c>
-      <c r="C44" s="11"/>
+        <v>74</v>
+      </c>
+      <c r="C44" s="13"/>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
@@ -3129,8 +3135,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3239,16 +3245,16 @@
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3257,13 +3263,13 @@
       <c r="A10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="12" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3272,18 +3278,31 @@
       <c r="A12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>